<commit_message>
condidates collector correction: there was y instead of h
</commit_message>
<xml_diff>
--- a/candidate_search/construction_examples-hardware.xlsx
+++ b/candidate_search/construction_examples-hardware.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\candidate_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4362733A-4A6A-4166-ABE6-6233F5D77116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D20C392-F1A5-4146-A7E8-6233B34C8F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>ExampleNum</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>C_hw_3</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -167,12 +167,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,8 +193,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -505,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AH20" sqref="AH20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -534,136 +541,136 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
       <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:45">
@@ -2310,140 +2317,140 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
-      <c r="A14">
+    <row r="14" spans="1:45" s="1" customFormat="1">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>32</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1">
         <v>64</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>-2</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>12</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>-5</v>
       </c>
-      <c r="G14">
-        <v>32</v>
-      </c>
-      <c r="H14">
+      <c r="G14" s="1">
+        <v>32</v>
+      </c>
+      <c r="H14" s="1">
         <v>44</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>42</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>-90</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>192</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>46</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>-64</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <v>-5</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <v>-35</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="1">
         <v>-6</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="1">
         <v>-2</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="1">
         <v>-9</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="1">
         <v>11</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="1">
         <v>-7</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="1">
         <v>46</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="1">
         <v>66</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="1">
         <v>48</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="1">
         <v>-12</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="1">
         <v>-7</v>
       </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
         <v>129</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="1">
         <v>134</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="1">
         <v>140</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="1">
         <v>52</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="1">
         <v>257</v>
       </c>
-      <c r="AF14">
+      <c r="AF14" s="1">
         <v>40</v>
       </c>
-      <c r="AG14">
+      <c r="AG14" s="1">
         <v>20826</v>
       </c>
-      <c r="AH14">
+      <c r="AH14" s="1">
         <v>24641</v>
       </c>
-      <c r="AI14">
+      <c r="AI14" s="1">
         <v>24125</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="1">
         <v>776</v>
       </c>
-      <c r="AK14">
+      <c r="AK14" s="1">
         <v>2141</v>
       </c>
-      <c r="AL14">
+      <c r="AL14" s="1">
         <v>788</v>
       </c>
-      <c r="AM14">
+      <c r="AM14" s="1">
         <v>23722</v>
       </c>
-      <c r="AN14">
+      <c r="AN14" s="1">
         <v>28697</v>
       </c>
-      <c r="AO14">
+      <c r="AO14" s="1">
         <v>27053</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" s="1">
         <v>40</v>
       </c>
-      <c r="AQ14">
+      <c r="AQ14" s="1">
         <v>3</v>
       </c>
-      <c r="AR14">
-        <v>1</v>
-      </c>
-      <c r="AS14">
+      <c r="AR14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>